<commit_message>
Full Automation a a FDR calculation by excel Sheet
</commit_message>
<xml_diff>
--- a/TestData/FDRCalculation.xlsx
+++ b/TestData/FDRCalculation.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9289165-FB38-4C66-A43A-19D2466DABB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C5918791-3DF7-404E-989E-10880579C922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Principal</t>
   </si>
@@ -64,6 +60,12 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -79,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +104,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,15 +144,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +438,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +457,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
@@ -461,124 +475,134 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>20000</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>24000</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>40000</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>70000</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>50000</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>51250</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>75000</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>76500</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>75000</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>75045.320000000007</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>